<commit_message>
added SphericalKMeans into ExtractorComponent
</commit_message>
<xml_diff>
--- a/scraper/project_diary.xlsx
+++ b/scraper/project_diary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Design Patterns</t>
   </si>
@@ -98,10 +98,16 @@
     <t xml:space="preserve">Develop a metric to select top k text nodes from a corpus</t>
   </si>
   <si>
+    <t xml:space="preserve">Jan 13, 2026</t>
+  </si>
+  <si>
     <t xml:space="preserve">Title-body content relevancy grade</t>
   </si>
   <si>
     <t xml:space="preserve">Develop another metric to aggregate the two similarity scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 14, 2026</t>
   </si>
   <si>
     <t xml:space="preserve">Clustering strategy</t>
@@ -118,11 +124,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,6 +151,29 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,80 +260,92 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -438,91 +480,91 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -542,84 +584,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="15.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="23.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="55.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="15.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="55.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2" t="s">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="17" t="n">
+      <c r="E3" s="18" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="14"/>
-      <c r="C4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="D4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="11" t="n">
         <v>0.9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14"/>
-      <c r="C5" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="A5" s="19" t="s">
         <v>28</v>
       </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="11" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>